<commit_message>
add github description to appendix and move figures too
</commit_message>
<xml_diff>
--- a/docs/data_mismatch.xlsx
+++ b/docs/data_mismatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksa\Documents\B.Sc\Abschlussarbeit\mrs-thesis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98E8019-04F8-487C-B8DE-0A75D8B2601D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7194A7E-3BC8-49E9-966B-F22A9B03606D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{FFE340D8-0315-4C87-AAC6-0E7F7FD9E17F}"/>
   </bookViews>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CFDBD46-37CD-41D9-9C37-D5F8B59E713E}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +956,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>45</v>

</xml_diff>